<commit_message>
use cases - config
</commit_message>
<xml_diff>
--- a/doc/Use-Case.xlsx
+++ b/doc/Use-Case.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Erasmus\RI\prácticas\ras-apuestas\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FE59ED-6884-481F-BAB8-46D6BA50DE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,109 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+  <si>
+    <t>Registro de usuario nuevo</t>
+  </si>
+  <si>
+    <t>Introduce los campos necesarios</t>
+  </si>
+  <si>
+    <t>Clica a registrarse</t>
+  </si>
+  <si>
+    <t>Se inicia sesión automáticamente</t>
+  </si>
+  <si>
+    <t>Excepción</t>
+  </si>
+  <si>
+    <t>(paso1)</t>
+  </si>
+  <si>
+    <t>Los campos no están en formato correcto</t>
+  </si>
+  <si>
+    <t>Regresa paso 1</t>
+  </si>
+  <si>
+    <t>El email ya está en uso</t>
+  </si>
+  <si>
+    <t>Inicio de sesión</t>
+  </si>
+  <si>
+    <t>Clica en iniciar sesión</t>
+  </si>
+  <si>
+    <t>El usuario inicia sesión y  accede a la página principal</t>
+  </si>
+  <si>
+    <t>Accede a la página principal</t>
+  </si>
+  <si>
+    <t>El usuario no existe</t>
+  </si>
+  <si>
+    <t>Realizar apuesta</t>
+  </si>
+  <si>
+    <t>Accede a una apuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduce la cantidad a apostar </t>
+  </si>
+  <si>
+    <t>Elige la apuesta</t>
+  </si>
+  <si>
+    <t>Confirma la apuesta</t>
+  </si>
+  <si>
+    <t>Se le redirige a una página con sus apuestas</t>
+  </si>
+  <si>
+    <t>(paso2)</t>
+  </si>
+  <si>
+    <t>El dinero apostado excede la cantidad del cliente</t>
+  </si>
+  <si>
+    <t>Regresa paso 2</t>
+  </si>
+  <si>
+    <t>Consultar apuestas</t>
+  </si>
+  <si>
+    <t>Accede a una lista de las apuestas propias</t>
+  </si>
+  <si>
+    <t>Comprueba el estado de la apuesta</t>
+  </si>
+  <si>
+    <t>Notificación fin apuesta</t>
+  </si>
+  <si>
+    <t>El usuario recibe una notificación con el resultado de una apuesta</t>
+  </si>
+  <si>
+    <t>El usuario clica en cobrar en aquellas apuestas ganadoras</t>
+  </si>
+  <si>
+    <t>El dinero es ingresado en el perfil del cliente</t>
+  </si>
+  <si>
+    <t>Visualizar apuestas</t>
+  </si>
+  <si>
+    <t>El usuario dispone de una lista de las apuestas disponibles</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +440,314 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>